<commit_message>
revision of causes also done
</commit_message>
<xml_diff>
--- a/revised/causes.xlsx
+++ b/revised/causes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51AA3C9-50BD-4C44-9F3C-089D5756DE1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD07E19-BD80-401B-A129-21AC65825D90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mechanical" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
-  <si>
-    <t>Mechanical Defects</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <r>
       <t xml:space="preserve"> </t>
@@ -126,9 +123,6 @@
   </si>
   <si>
     <t>No of Accidents</t>
-  </si>
-  <si>
-    <t>cause of accidents due to signal defects</t>
   </si>
   <si>
     <t>Point Gaping</t>
@@ -220,7 +214,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -243,6 +237,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -254,41 +259,29 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -303,6 +296,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -586,130 +585,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A2:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="26">
-      <c r="A1" s="4" t="s">
+    <row r="2" spans="1:15" ht="117">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="39">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="104">
-      <c r="A3" s="1" t="s">
+      <c r="J2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7">
+        <v>3</v>
+      </c>
+      <c r="D3" s="7">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="39">
-      <c r="A4" s="5" t="s">
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7">
+        <v>5</v>
+      </c>
+      <c r="K3" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="78">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="117">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="3">
+        <v>8</v>
+      </c>
+      <c r="N3" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="39">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="39">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="39">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="52">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="42">
-      <c r="A14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="28">
-      <c r="A15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6">
-        <v>2</v>
+      <c r="O3" s="14">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -719,75 +694,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E682763A-59F5-4553-9B3D-B869BDFDDC32}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="65">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" ht="52">
+      <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="26">
-      <c r="A2" s="12" t="s">
+      <c r="C1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10">
+      <c r="D1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="26">
-      <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="10">
+      <c r="B2" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="39">
-      <c r="A4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10">
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="26">
-      <c r="A5" s="9" t="s">
+      <c r="D2" s="7">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14">
         <v>20</v>
       </c>
-      <c r="B5" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="39">
-      <c r="A6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="26">
-      <c r="A7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="52">
-      <c r="A8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="10">
-        <v>1</v>
-      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -798,107 +797,107 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7738A1-E8F9-4C6B-8138-336AD415C5AD}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4" ht="75">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>15</v>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5">
-      <c r="A2" s="14">
+      <c r="A2" s="10">
         <v>2016</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="10">
         <v>24</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="12">
         <v>6</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="12">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5">
-      <c r="A3" s="14">
+      <c r="A3" s="10">
         <v>2017</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>5</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="12">
         <v>3</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.5">
-      <c r="A4" s="14">
+      <c r="A4" s="10">
         <v>2018</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>11</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="12">
         <v>3</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.5">
-      <c r="A5" s="14">
+      <c r="A5" s="10">
         <v>2019</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>18</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="12">
         <v>5</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5">
-      <c r="A6" s="14">
+      <c r="A6" s="10">
         <v>2020</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="10">
         <v>8</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="12">
         <v>7</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.5">
-      <c r="A7" s="14">
+      <c r="A7" s="10">
         <v>2021</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="10">
         <v>9</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="12">
         <v>10</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="12">
         <v>3</v>
       </c>
     </row>

</xml_diff>